<commit_message>
HHR maps being displayed, but to be complete
</commit_message>
<xml_diff>
--- a/src/geohubsql/sql/plpgsql/GeoHub_layer_registration.xlsx
+++ b/src/geohubsql/sql/plpgsql/GeoHub_layer_registration.xlsx
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="32">
+  <si>
+    <t xml:space="preserve">https://github.com/UNDP-Data/geohub/pull/1556</t>
+  </si>
   <si>
     <t xml:space="preserve">TAGS</t>
   </si>
@@ -104,21 +107,30 @@
   </si>
   <si>
     <t xml:space="preserve">Subnational Mean years of schooling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">drr.dynamic_subnational_hhr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8c4810867c50ee006b11abf19876a750</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subnational Heat Health Risk</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
   <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -136,12 +148,18 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -184,20 +202,28 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -278,639 +304,790 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A3:K41"/>
+  <dimension ref="A1:K51"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D7:M8"/>
+      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="63.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="82.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="77.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="296.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="200.27"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="1" t="str">
+        <f aca="false">"https://pgtileserv.undpgeohub.org/"</f>
+        <v>https://pgtileserv.undpgeohub.org/</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C3" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="F3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="0" t="str">
-        <f aca="false">""</f>
-        <v/>
-      </c>
-      <c r="K3" s="0" t="s">
+      <c r="G3" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I3" s="1" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="F4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="0" t="str">
+      <c r="G4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="1" t="str">
         <f aca="false">""</f>
         <v/>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I5" s="0" t="str">
+      <c r="I5" s="1" t="str">
         <f aca="false">""</f>
         <v/>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="0" t="str">
+      <c r="B6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="1" t="str">
         <f aca="false">""</f>
         <v/>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="0" t="str">
-        <f aca="false">"http://172.18.0.6:7800/"&amp;B6&amp;"/{z}/{x}/{y}.pbf"</f>
-        <v>http://172.18.0.6:7800/admin.subnational_gross_national_income/{z}/{x}/{y}.pbf</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="0" t="str">
-        <f aca="false">""</f>
-        <v/>
-      </c>
-      <c r="E7" s="0" t="str">
-        <f aca="false">""</f>
-        <v/>
-      </c>
-      <c r="F7" s="0" t="str">
-        <f aca="false">""</f>
-        <v/>
-      </c>
-      <c r="G7" s="0" t="str">
-        <f aca="false">""</f>
-        <v/>
-      </c>
-      <c r="I7" s="0" t="str">
-        <f aca="false">""</f>
-        <v/>
-      </c>
-      <c r="K7" s="2" t="str">
+      <c r="B7" s="1" t="str">
+        <f aca="false">$B$1&amp;B6&amp;"/{z}/{x}/{y}.pbf"</f>
+        <v>https://pgtileserv.undpgeohub.org/admin.subnational_gross_national_income/{z}/{x}/{y}.pbf</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="1" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="E7" s="1" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="F7" s="1" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="G7" s="1" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="I7" s="1" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="K7" s="4" t="str">
         <f aca="false">"INSERT INTO geohub.tag (key, value) SELECT '"&amp;K$3&amp;"', '"&amp;$B6&amp;"' WHERE NOT EXISTS (SELECT key,value FROM geohub.tag WHERE key='"&amp;K$3&amp;"' AND value='"&amp;B6&amp;"');"</f>
         <v>INSERT INTO geohub.tag (key, value) SELECT 'id', 'admin.subnational_gross_national_income' WHERE NOT EXISTS (SELECT key,value FROM geohub.tag WHERE key='id' AND value='admin.subnational_gross_national_income');</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="3" t="str">
+      <c r="B8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="5" t="str">
         <f aca="false">"VALUES ('"&amp;B8&amp;"', '"&amp;B7&amp;"', False, 'Creative Commons BY NonCommercial ShareAlike 4.0', (SELECT ST_SetSRID(ST_Extent(geom),4326)  AS geom FROM admin.admin0), current_timestamp, current_timestamp, '"&amp;B9&amp;"', '"&amp;B9&amp;"', 'douglas.tommasi@undp.org', 'douglas.tommasi@undp.org');"</f>
-        <v>VALUES ('b35c09fd8fc981d388381dddc146713c', 'http://172.18.0.6:7800/admin.subnational_gross_national_income/{z}/{x}/{y}.pbf', False, 'Creative Commons BY NonCommercial ShareAlike 4.0', (SELECT ST_SetSRID(ST_Extent(geom),4326)  AS geom FROM admin.admin0), current_timestamp, current_timestamp, 'Subnational Gross National Income per capita', 'Subnational Gross National Income per capita', 'douglas.tommasi@undp.org', 'douglas.tommasi@undp.org');</v>
-      </c>
-      <c r="D8" s="0" t="str">
+        <v>VALUES ('b35c09fd8fc981d388381dddc146713c', 'https://pgtileserv.undpgeohub.org/admin.subnational_gross_national_income/{z}/{x}/{y}.pbf', False, 'Creative Commons BY NonCommercial ShareAlike 4.0', (SELECT ST_SetSRID(ST_Extent(geom),4326)  AS geom FROM admin.admin0), current_timestamp, current_timestamp, 'Subnational Gross National Income per capita', 'Subnational Gross National Income per capita', 'douglas.tommasi@undp.org', 'douglas.tommasi@undp.org');</v>
+      </c>
+      <c r="D8" s="1" t="str">
         <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B8&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;D$3&amp;"' AND value='"&amp;D$4&amp;"'))  ON CONFLICT DO NOTHING;"</f>
         <v>INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('b35c09fd8fc981d388381dddc146713c',(SELECT id FROM geohub.tag WHERE key='type' AND value='pgtileserv'))  ON CONFLICT DO NOTHING;</v>
       </c>
-      <c r="E8" s="0" t="str">
+      <c r="E8" s="1" t="str">
         <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B8&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;E$3&amp;"' AND value='"&amp;E$4&amp;"'))  ON CONFLICT DO NOTHING;"</f>
         <v>INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('b35c09fd8fc981d388381dddc146713c',(SELECT id FROM geohub.tag WHERE key='layertype' AND value='function'))  ON CONFLICT DO NOTHING;</v>
       </c>
-      <c r="F8" s="0" t="str">
+      <c r="F8" s="1" t="str">
         <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B8&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;F$3&amp;"' AND value='"&amp;F$4&amp;"'))  ON CONFLICT DO NOTHING;"</f>
         <v>INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('b35c09fd8fc981d388381dddc146713c',(SELECT id FROM geohub.tag WHERE key='extent' AND value='Global'))  ON CONFLICT DO NOTHING;</v>
       </c>
-      <c r="G8" s="0" t="str">
+      <c r="G8" s="1" t="str">
         <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B8&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;G$3&amp;"' AND value='"&amp;G$4&amp;"'))  ON CONFLICT DO NOTHING;"</f>
         <v>INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('b35c09fd8fc981d388381dddc146713c',(SELECT id FROM geohub.tag WHERE key='geometrytype' AND value='MultiPolygon'))  ON CONFLICT DO NOTHING;</v>
       </c>
-      <c r="I8" s="0" t="str">
-        <f aca="false">""</f>
-        <v/>
-      </c>
-      <c r="K8" s="0" t="str">
+      <c r="I8" s="1" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="K8" s="1" t="str">
         <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B8&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;K$3&amp;"' AND value='"&amp;$B6&amp;"'))  ON CONFLICT DO NOTHING;"</f>
         <v>INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('b35c09fd8fc981d388381dddc146713c',(SELECT id FROM geohub.tag WHERE key='id' AND value='admin.subnational_gross_national_income'))  ON CONFLICT DO NOTHING;</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="0" t="str">
+      <c r="B9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="1" t="str">
         <f aca="false">"--DELETE FROM geohub.dataset WHERE id ='"&amp;B8&amp;"';"</f>
         <v>--DELETE FROM geohub.dataset WHERE id ='b35c09fd8fc981d388381dddc146713c';</v>
       </c>
-      <c r="D9" s="0" t="str">
+      <c r="D9" s="1" t="str">
         <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B8&amp;"';"</f>
         <v>--DELETE FROM geohub.dataset_tag WHERE dataset_id='b35c09fd8fc981d388381dddc146713c';</v>
       </c>
-      <c r="E9" s="0" t="str">
+      <c r="E9" s="1" t="str">
         <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B8&amp;"';"</f>
         <v>--DELETE FROM geohub.dataset_tag WHERE dataset_id='b35c09fd8fc981d388381dddc146713c';</v>
       </c>
-      <c r="F9" s="0" t="str">
+      <c r="F9" s="1" t="str">
         <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B8&amp;"';"</f>
         <v>--DELETE FROM geohub.dataset_tag WHERE dataset_id='b35c09fd8fc981d388381dddc146713c';</v>
       </c>
-      <c r="G9" s="0" t="str">
+      <c r="G9" s="1" t="str">
         <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B8&amp;"';"</f>
         <v>--DELETE FROM geohub.dataset_tag WHERE dataset_id='b35c09fd8fc981d388381dddc146713c';</v>
       </c>
-      <c r="I9" s="0" t="str">
-        <f aca="false">""</f>
-        <v/>
-      </c>
-      <c r="K9" s="0" t="str">
+      <c r="I9" s="1" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="K9" s="1" t="str">
         <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B8&amp;"';"</f>
         <v>--DELETE FROM geohub.dataset_tag WHERE dataset_id='b35c09fd8fc981d388381dddc146713c';</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I10" s="0" t="str">
+      <c r="I10" s="1" t="str">
         <f aca="false">""</f>
         <v/>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="3" t="str">
+      <c r="B11" s="5" t="str">
         <f aca="false">"echo -n '"&amp;B7&amp;"'|md5sum"</f>
-        <v>echo -n 'http://172.18.0.6:7800/admin.subnational_gross_national_income/{z}/{x}/{y}.pbf'|md5sum</v>
-      </c>
-      <c r="I11" s="0" t="str">
+        <v>echo -n 'https://pgtileserv.undpgeohub.org/admin.subnational_gross_national_income/{z}/{x}/{y}.pbf'|md5sum</v>
+      </c>
+      <c r="I11" s="1" t="str">
         <f aca="false">""</f>
         <v/>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I12" s="0" t="str">
+      <c r="I12" s="1" t="str">
         <f aca="false">""</f>
         <v/>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I13" s="0" t="str">
+      <c r="I13" s="1" t="str">
         <f aca="false">""</f>
         <v/>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I14" s="0" t="str">
+      <c r="I14" s="1" t="str">
         <f aca="false">""</f>
         <v/>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I15" s="0" t="str">
+      <c r="I15" s="1" t="str">
         <f aca="false">""</f>
         <v/>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I16" s="0" t="str">
+      <c r="I16" s="1" t="str">
         <f aca="false">""</f>
         <v/>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I17" s="0" t="str">
+      <c r="A17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I17" s="1" t="str">
         <f aca="false">""</f>
         <v/>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="2" t="str">
-        <f aca="false">"http://172.18.0.6:7800/"&amp;B17&amp;"/{z}/{x}/{y}.pbf"</f>
-        <v>http://172.18.0.6:7800/admin.subnational_life_expectancy/{z}/{x}/{y}.pbf</v>
-      </c>
-      <c r="C18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="0" t="str">
-        <f aca="false">""</f>
-        <v/>
-      </c>
-      <c r="E18" s="0" t="str">
-        <f aca="false">""</f>
-        <v/>
-      </c>
-      <c r="F18" s="0" t="str">
-        <f aca="false">""</f>
-        <v/>
-      </c>
-      <c r="G18" s="0" t="str">
-        <f aca="false">""</f>
-        <v/>
-      </c>
-      <c r="I18" s="0" t="str">
-        <f aca="false">""</f>
-        <v/>
-      </c>
-      <c r="K18" s="0" t="str">
+      <c r="B18" s="1" t="str">
+        <f aca="false">$B$1&amp;B17&amp;"/{z}/{x}/{y}.pbf"</f>
+        <v>https://pgtileserv.undpgeohub.org/admin.subnational_life_expectancy/{z}/{x}/{y}.pbf</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="1" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="E18" s="1" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="F18" s="1" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="G18" s="1" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="I18" s="1" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="K18" s="1" t="str">
         <f aca="false">"INSERT INTO geohub.tag (key, value) SELECT '"&amp;K$3&amp;"', '"&amp;$B17&amp;"' WHERE NOT EXISTS (SELECT key,value FROM geohub.tag WHERE key='"&amp;K$3&amp;"' AND value='"&amp;B17&amp;"');"</f>
         <v>INSERT INTO geohub.tag (key, value) SELECT 'id', 'admin.subnational_life_expectancy' WHERE NOT EXISTS (SELECT key,value FROM geohub.tag WHERE key='id' AND value='admin.subnational_life_expectancy');</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="3" t="str">
+      <c r="A19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="5" t="str">
         <f aca="false">"VALUES ('"&amp;B19&amp;"', '"&amp;B18&amp;"', False, 'Creative Commons BY NonCommercial ShareAlike 4.0', (SELECT ST_SetSRID(ST_Extent(geom),4326)  AS geom FROM admin.admin0), current_timestamp, current_timestamp, '"&amp;B20&amp;"', '"&amp;B20&amp;"', 'douglas.tommasi@undp.org', 'douglas.tommasi@undp.org');"</f>
-        <v>VALUES ('3b0a0ed77b9560c8047a9b9c0313cb0a', 'http://172.18.0.6:7800/admin.subnational_life_expectancy/{z}/{x}/{y}.pbf', False, 'Creative Commons BY NonCommercial ShareAlike 4.0', (SELECT ST_SetSRID(ST_Extent(geom),4326)  AS geom FROM admin.admin0), current_timestamp, current_timestamp, 'Subnational Life Expectancy', 'Subnational Life Expectancy', 'douglas.tommasi@undp.org', 'douglas.tommasi@undp.org');</v>
-      </c>
-      <c r="D19" s="0" t="str">
+        <v>VALUES ('3b0a0ed77b9560c8047a9b9c0313cb0a', 'https://pgtileserv.undpgeohub.org/admin.subnational_life_expectancy/{z}/{x}/{y}.pbf', False, 'Creative Commons BY NonCommercial ShareAlike 4.0', (SELECT ST_SetSRID(ST_Extent(geom),4326)  AS geom FROM admin.admin0), current_timestamp, current_timestamp, 'Subnational Life Expectancy', 'Subnational Life Expectancy', 'douglas.tommasi@undp.org', 'douglas.tommasi@undp.org');</v>
+      </c>
+      <c r="D19" s="1" t="str">
         <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B19&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;D$3&amp;"' AND value='"&amp;D$4&amp;"'))  ON CONFLICT DO NOTHING;"</f>
         <v>INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('3b0a0ed77b9560c8047a9b9c0313cb0a',(SELECT id FROM geohub.tag WHERE key='type' AND value='pgtileserv'))  ON CONFLICT DO NOTHING;</v>
       </c>
-      <c r="E19" s="0" t="str">
+      <c r="E19" s="1" t="str">
         <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B19&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;E$3&amp;"' AND value='"&amp;E$4&amp;"'))  ON CONFLICT DO NOTHING;"</f>
         <v>INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('3b0a0ed77b9560c8047a9b9c0313cb0a',(SELECT id FROM geohub.tag WHERE key='layertype' AND value='function'))  ON CONFLICT DO NOTHING;</v>
       </c>
-      <c r="F19" s="0" t="str">
+      <c r="F19" s="1" t="str">
         <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B19&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;F$3&amp;"' AND value='"&amp;F$4&amp;"'))  ON CONFLICT DO NOTHING;"</f>
         <v>INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('3b0a0ed77b9560c8047a9b9c0313cb0a',(SELECT id FROM geohub.tag WHERE key='extent' AND value='Global'))  ON CONFLICT DO NOTHING;</v>
       </c>
-      <c r="G19" s="0" t="str">
+      <c r="G19" s="1" t="str">
         <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B19&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;G$3&amp;"' AND value='"&amp;G$4&amp;"'))  ON CONFLICT DO NOTHING;"</f>
         <v>INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('3b0a0ed77b9560c8047a9b9c0313cb0a',(SELECT id FROM geohub.tag WHERE key='geometrytype' AND value='MultiPolygon'))  ON CONFLICT DO NOTHING;</v>
       </c>
-      <c r="I19" s="0" t="str">
-        <f aca="false">""</f>
-        <v/>
-      </c>
-      <c r="K19" s="0" t="str">
+      <c r="I19" s="1" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="K19" s="1" t="str">
         <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B19&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;K$3&amp;"' AND value='"&amp;$B17&amp;"'))  ON CONFLICT DO NOTHING;"</f>
         <v>INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('3b0a0ed77b9560c8047a9b9c0313cb0a',(SELECT id FROM geohub.tag WHERE key='id' AND value='admin.subnational_life_expectancy'))  ON CONFLICT DO NOTHING;</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="0" t="str">
+      <c r="A20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="1" t="str">
         <f aca="false">"--DELETE FROM geohub.dataset WHERE id ='"&amp;B19&amp;"';"</f>
         <v>--DELETE FROM geohub.dataset WHERE id ='3b0a0ed77b9560c8047a9b9c0313cb0a';</v>
       </c>
-      <c r="D20" s="0" t="str">
+      <c r="D20" s="1" t="str">
         <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B19&amp;"';"</f>
         <v>--DELETE FROM geohub.dataset_tag WHERE dataset_id='3b0a0ed77b9560c8047a9b9c0313cb0a';</v>
       </c>
-      <c r="E20" s="0" t="str">
+      <c r="E20" s="1" t="str">
         <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B19&amp;"';"</f>
         <v>--DELETE FROM geohub.dataset_tag WHERE dataset_id='3b0a0ed77b9560c8047a9b9c0313cb0a';</v>
       </c>
-      <c r="F20" s="0" t="str">
+      <c r="F20" s="1" t="str">
         <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B19&amp;"';"</f>
         <v>--DELETE FROM geohub.dataset_tag WHERE dataset_id='3b0a0ed77b9560c8047a9b9c0313cb0a';</v>
       </c>
-      <c r="G20" s="0" t="str">
+      <c r="G20" s="1" t="str">
         <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B19&amp;"';"</f>
         <v>--DELETE FROM geohub.dataset_tag WHERE dataset_id='3b0a0ed77b9560c8047a9b9c0313cb0a';</v>
       </c>
-      <c r="I20" s="0" t="str">
-        <f aca="false">""</f>
-        <v/>
-      </c>
-      <c r="K20" s="0" t="str">
+      <c r="I20" s="1" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="K20" s="1" t="str">
         <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B19&amp;"';"</f>
         <v>--DELETE FROM geohub.dataset_tag WHERE dataset_id='3b0a0ed77b9560c8047a9b9c0313cb0a';</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I21" s="0" t="str">
+      <c r="I21" s="1" t="str">
         <f aca="false">""</f>
         <v/>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="3" t="str">
+      <c r="B22" s="5" t="str">
         <f aca="false">"echo -n '"&amp;B18&amp;"'|md5sum"</f>
-        <v>echo -n 'http://172.18.0.6:7800/admin.subnational_life_expectancy/{z}/{x}/{y}.pbf'|md5sum</v>
-      </c>
-      <c r="I22" s="0" t="str">
+        <v>echo -n 'https://pgtileserv.undpgeohub.org/admin.subnational_life_expectancy/{z}/{x}/{y}.pbf'|md5sum</v>
+      </c>
+      <c r="I22" s="1" t="str">
         <f aca="false">""</f>
         <v/>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I28" s="0" t="str">
+      <c r="A28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I28" s="1" t="str">
         <f aca="false">""</f>
         <v/>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B29" s="2" t="str">
-        <f aca="false">"http://172.18.0.6:7800/"&amp;B28&amp;"/{z}/{x}/{y}.pbf"</f>
-        <v>http://172.18.0.6:7800/admin.subnational_expected_years_of_schooling/{z}/{x}/{y}.pbf</v>
-      </c>
-      <c r="C29" s="2" t="s">
+      <c r="A29" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D29" s="0" t="str">
-        <f aca="false">""</f>
-        <v/>
-      </c>
-      <c r="E29" s="0" t="str">
-        <f aca="false">""</f>
-        <v/>
-      </c>
-      <c r="F29" s="0" t="str">
-        <f aca="false">""</f>
-        <v/>
-      </c>
-      <c r="G29" s="0" t="str">
-        <f aca="false">""</f>
-        <v/>
-      </c>
-      <c r="I29" s="0" t="str">
-        <f aca="false">""</f>
-        <v/>
-      </c>
-      <c r="K29" s="0" t="str">
+      <c r="B29" s="1" t="str">
+        <f aca="false">$B$1&amp;B28&amp;"/{z}/{x}/{y}.pbf"</f>
+        <v>https://pgtileserv.undpgeohub.org/admin.subnational_expected_years_of_schooling/{z}/{x}/{y}.pbf</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" s="1" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="E29" s="1" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="F29" s="1" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="G29" s="1" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="I29" s="1" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="K29" s="1" t="str">
         <f aca="false">"INSERT INTO geohub.tag (key, value) SELECT '"&amp;K$3&amp;"', '"&amp;$B28&amp;"' WHERE NOT EXISTS (SELECT key,value FROM geohub.tag WHERE key='"&amp;K$3&amp;"' AND value='"&amp;B28&amp;"');"</f>
         <v>INSERT INTO geohub.tag (key, value) SELECT 'id', 'admin.subnational_expected_years_of_schooling' WHERE NOT EXISTS (SELECT key,value FROM geohub.tag WHERE key='id' AND value='admin.subnational_expected_years_of_schooling');</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C30" s="3" t="str">
+      <c r="A30" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="5" t="str">
         <f aca="false">"VALUES ('"&amp;B30&amp;"', '"&amp;B29&amp;"', False, 'Creative Commons BY NonCommercial ShareAlike 4.0', (SELECT ST_SetSRID(ST_Extent(geom),4326)  AS geom FROM admin.admin0), current_timestamp, current_timestamp, '"&amp;B31&amp;"', '"&amp;B31&amp;"', 'douglas.tommasi@undp.org', 'douglas.tommasi@undp.org');"</f>
-        <v>VALUES ('571be599e1cc42752265fc7652f296de', 'http://172.18.0.6:7800/admin.subnational_expected_years_of_schooling/{z}/{x}/{y}.pbf', False, 'Creative Commons BY NonCommercial ShareAlike 4.0', (SELECT ST_SetSRID(ST_Extent(geom),4326)  AS geom FROM admin.admin0), current_timestamp, current_timestamp, 'Subnational Expected years of schooling', 'Subnational Expected years of schooling', 'douglas.tommasi@undp.org', 'douglas.tommasi@undp.org');</v>
-      </c>
-      <c r="D30" s="0" t="str">
+        <v>VALUES ('571be599e1cc42752265fc7652f296de', 'https://pgtileserv.undpgeohub.org/admin.subnational_expected_years_of_schooling/{z}/{x}/{y}.pbf', False, 'Creative Commons BY NonCommercial ShareAlike 4.0', (SELECT ST_SetSRID(ST_Extent(geom),4326)  AS geom FROM admin.admin0), current_timestamp, current_timestamp, 'Subnational Expected years of schooling', 'Subnational Expected years of schooling', 'douglas.tommasi@undp.org', 'douglas.tommasi@undp.org');</v>
+      </c>
+      <c r="D30" s="1" t="str">
         <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B30&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;D$3&amp;"' AND value='"&amp;D$4&amp;"'))  ON CONFLICT DO NOTHING;"</f>
         <v>INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('571be599e1cc42752265fc7652f296de',(SELECT id FROM geohub.tag WHERE key='type' AND value='pgtileserv'))  ON CONFLICT DO NOTHING;</v>
       </c>
-      <c r="E30" s="0" t="str">
+      <c r="E30" s="1" t="str">
         <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B30&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;E$3&amp;"' AND value='"&amp;E$4&amp;"'))  ON CONFLICT DO NOTHING;"</f>
         <v>INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('571be599e1cc42752265fc7652f296de',(SELECT id FROM geohub.tag WHERE key='layertype' AND value='function'))  ON CONFLICT DO NOTHING;</v>
       </c>
-      <c r="F30" s="0" t="str">
+      <c r="F30" s="1" t="str">
         <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B30&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;F$3&amp;"' AND value='"&amp;F$4&amp;"'))  ON CONFLICT DO NOTHING;"</f>
         <v>INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('571be599e1cc42752265fc7652f296de',(SELECT id FROM geohub.tag WHERE key='extent' AND value='Global'))  ON CONFLICT DO NOTHING;</v>
       </c>
-      <c r="G30" s="0" t="str">
+      <c r="G30" s="1" t="str">
         <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B30&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;G$3&amp;"' AND value='"&amp;G$4&amp;"'))  ON CONFLICT DO NOTHING;"</f>
         <v>INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('571be599e1cc42752265fc7652f296de',(SELECT id FROM geohub.tag WHERE key='geometrytype' AND value='MultiPolygon'))  ON CONFLICT DO NOTHING;</v>
       </c>
-      <c r="I30" s="0" t="str">
-        <f aca="false">""</f>
-        <v/>
-      </c>
-      <c r="K30" s="0" t="str">
+      <c r="I30" s="1" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="K30" s="1" t="str">
         <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B30&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;K$3&amp;"' AND value='"&amp;$B28&amp;"'))  ON CONFLICT DO NOTHING;"</f>
         <v>INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('571be599e1cc42752265fc7652f296de',(SELECT id FROM geohub.tag WHERE key='id' AND value='admin.subnational_expected_years_of_schooling'))  ON CONFLICT DO NOTHING;</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B31" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C31" s="0" t="str">
+      <c r="A31" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" s="1" t="str">
         <f aca="false">"--DELETE FROM geohub.dataset WHERE id ='"&amp;B30&amp;"';"</f>
         <v>--DELETE FROM geohub.dataset WHERE id ='571be599e1cc42752265fc7652f296de';</v>
       </c>
-      <c r="D31" s="0" t="str">
+      <c r="D31" s="1" t="str">
         <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B30&amp;"';"</f>
         <v>--DELETE FROM geohub.dataset_tag WHERE dataset_id='571be599e1cc42752265fc7652f296de';</v>
       </c>
-      <c r="E31" s="0" t="str">
+      <c r="E31" s="1" t="str">
         <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B30&amp;"';"</f>
         <v>--DELETE FROM geohub.dataset_tag WHERE dataset_id='571be599e1cc42752265fc7652f296de';</v>
       </c>
-      <c r="F31" s="0" t="str">
+      <c r="F31" s="1" t="str">
         <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B30&amp;"';"</f>
         <v>--DELETE FROM geohub.dataset_tag WHERE dataset_id='571be599e1cc42752265fc7652f296de';</v>
       </c>
-      <c r="G31" s="0" t="str">
+      <c r="G31" s="1" t="str">
         <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B30&amp;"';"</f>
         <v>--DELETE FROM geohub.dataset_tag WHERE dataset_id='571be599e1cc42752265fc7652f296de';</v>
       </c>
-      <c r="I31" s="0" t="str">
-        <f aca="false">""</f>
-        <v/>
-      </c>
-      <c r="K31" s="0" t="str">
+      <c r="I31" s="1" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="K31" s="1" t="str">
         <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B30&amp;"';"</f>
         <v>--DELETE FROM geohub.dataset_tag WHERE dataset_id='571be599e1cc42752265fc7652f296de';</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I32" s="0" t="str">
+      <c r="I32" s="1" t="str">
         <f aca="false">""</f>
         <v/>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="3" t="str">
+      <c r="B33" s="5" t="str">
         <f aca="false">"echo -n '"&amp;B29&amp;"'|md5sum"</f>
-        <v>echo -n 'http://172.18.0.6:7800/admin.subnational_expected_years_of_schooling/{z}/{x}/{y}.pbf'|md5sum</v>
-      </c>
-      <c r="I33" s="0" t="str">
+        <v>echo -n 'https://pgtileserv.undpgeohub.org/admin.subnational_expected_years_of_schooling/{z}/{x}/{y}.pbf'|md5sum</v>
+      </c>
+      <c r="I33" s="1" t="str">
         <f aca="false">""</f>
         <v/>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I36" s="0" t="str">
+      <c r="A36" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I36" s="1" t="str">
         <f aca="false">""</f>
         <v/>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B37" s="2" t="str">
-        <f aca="false">"http://172.18.0.6:7800/"&amp;B36&amp;"/{z}/{x}/{y}.pbf"</f>
-        <v>http://172.18.0.6:7800/admin.subnational_mean_years_of_schooling/{z}/{x}/{y}.pbf</v>
-      </c>
-      <c r="C37" s="2" t="s">
+      <c r="A37" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D37" s="0" t="str">
-        <f aca="false">""</f>
-        <v/>
-      </c>
-      <c r="E37" s="0" t="str">
-        <f aca="false">""</f>
-        <v/>
-      </c>
-      <c r="F37" s="0" t="str">
-        <f aca="false">""</f>
-        <v/>
-      </c>
-      <c r="G37" s="0" t="str">
-        <f aca="false">""</f>
-        <v/>
-      </c>
-      <c r="I37" s="0" t="str">
-        <f aca="false">""</f>
-        <v/>
-      </c>
-      <c r="K37" s="0" t="str">
+      <c r="B37" s="1" t="str">
+        <f aca="false">$B$1&amp;B36&amp;"/{z}/{x}/{y}.pbf"</f>
+        <v>https://pgtileserv.undpgeohub.org/admin.subnational_mean_years_of_schooling/{z}/{x}/{y}.pbf</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37" s="1" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="E37" s="1" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="F37" s="1" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="G37" s="1" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="I37" s="1" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="K37" s="1" t="str">
         <f aca="false">"INSERT INTO geohub.tag (key, value) SELECT '"&amp;K$3&amp;"', '"&amp;$B36&amp;"' WHERE NOT EXISTS (SELECT key,value FROM geohub.tag WHERE key='"&amp;K$3&amp;"' AND value='"&amp;B36&amp;"');"</f>
         <v>INSERT INTO geohub.tag (key, value) SELECT 'id', 'admin.subnational_mean_years_of_schooling' WHERE NOT EXISTS (SELECT key,value FROM geohub.tag WHERE key='id' AND value='admin.subnational_mean_years_of_schooling');</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C38" s="3" t="str">
+      <c r="A38" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C38" s="5" t="str">
         <f aca="false">"VALUES ('"&amp;B38&amp;"', '"&amp;B37&amp;"', False, 'Creative Commons BY NonCommercial ShareAlike 4.0', (SELECT ST_SetSRID(ST_Extent(geom),4326)  AS geom FROM admin.admin0), current_timestamp, current_timestamp, '"&amp;B39&amp;"', '"&amp;B39&amp;"', 'douglas.tommasi@undp.org', 'douglas.tommasi@undp.org');"</f>
-        <v>VALUES ('99a374e15fd142049e247aee3b973c15', 'http://172.18.0.6:7800/admin.subnational_mean_years_of_schooling/{z}/{x}/{y}.pbf', False, 'Creative Commons BY NonCommercial ShareAlike 4.0', (SELECT ST_SetSRID(ST_Extent(geom),4326)  AS geom FROM admin.admin0), current_timestamp, current_timestamp, 'Subnational Mean years of schooling', 'Subnational Mean years of schooling', 'douglas.tommasi@undp.org', 'douglas.tommasi@undp.org');</v>
-      </c>
-      <c r="D38" s="0" t="str">
+        <v>VALUES ('99a374e15fd142049e247aee3b973c15', 'https://pgtileserv.undpgeohub.org/admin.subnational_mean_years_of_schooling/{z}/{x}/{y}.pbf', False, 'Creative Commons BY NonCommercial ShareAlike 4.0', (SELECT ST_SetSRID(ST_Extent(geom),4326)  AS geom FROM admin.admin0), current_timestamp, current_timestamp, 'Subnational Mean years of schooling', 'Subnational Mean years of schooling', 'douglas.tommasi@undp.org', 'douglas.tommasi@undp.org');</v>
+      </c>
+      <c r="D38" s="1" t="str">
         <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B38&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;D$3&amp;"' AND value='"&amp;D$4&amp;"'))  ON CONFLICT DO NOTHING;"</f>
         <v>INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('99a374e15fd142049e247aee3b973c15',(SELECT id FROM geohub.tag WHERE key='type' AND value='pgtileserv'))  ON CONFLICT DO NOTHING;</v>
       </c>
-      <c r="E38" s="0" t="str">
+      <c r="E38" s="1" t="str">
         <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B38&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;E$3&amp;"' AND value='"&amp;E$4&amp;"'))  ON CONFLICT DO NOTHING;"</f>
         <v>INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('99a374e15fd142049e247aee3b973c15',(SELECT id FROM geohub.tag WHERE key='layertype' AND value='function'))  ON CONFLICT DO NOTHING;</v>
       </c>
-      <c r="F38" s="0" t="str">
+      <c r="F38" s="1" t="str">
         <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B38&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;F$3&amp;"' AND value='"&amp;F$4&amp;"'))  ON CONFLICT DO NOTHING;"</f>
         <v>INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('99a374e15fd142049e247aee3b973c15',(SELECT id FROM geohub.tag WHERE key='extent' AND value='Global'))  ON CONFLICT DO NOTHING;</v>
       </c>
-      <c r="G38" s="0" t="str">
+      <c r="G38" s="1" t="str">
         <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B38&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;G$3&amp;"' AND value='"&amp;G$4&amp;"'))  ON CONFLICT DO NOTHING;"</f>
         <v>INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('99a374e15fd142049e247aee3b973c15',(SELECT id FROM geohub.tag WHERE key='geometrytype' AND value='MultiPolygon'))  ON CONFLICT DO NOTHING;</v>
       </c>
-      <c r="I38" s="0" t="str">
-        <f aca="false">""</f>
-        <v/>
-      </c>
-      <c r="K38" s="0" t="str">
+      <c r="I38" s="1" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="K38" s="1" t="str">
         <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B38&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;K$3&amp;"' AND value='"&amp;$B36&amp;"'))  ON CONFLICT DO NOTHING;"</f>
         <v>INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('99a374e15fd142049e247aee3b973c15',(SELECT id FROM geohub.tag WHERE key='id' AND value='admin.subnational_mean_years_of_schooling'))  ON CONFLICT DO NOTHING;</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B39" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="C39" s="0" t="str">
+      <c r="A39" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C39" s="1" t="str">
         <f aca="false">"--DELETE FROM geohub.dataset WHERE id ='"&amp;B38&amp;"';"</f>
         <v>--DELETE FROM geohub.dataset WHERE id ='99a374e15fd142049e247aee3b973c15';</v>
       </c>
-      <c r="D39" s="0" t="str">
+      <c r="D39" s="1" t="str">
         <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B38&amp;"';"</f>
         <v>--DELETE FROM geohub.dataset_tag WHERE dataset_id='99a374e15fd142049e247aee3b973c15';</v>
       </c>
-      <c r="E39" s="0" t="str">
+      <c r="E39" s="1" t="str">
         <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B38&amp;"';"</f>
         <v>--DELETE FROM geohub.dataset_tag WHERE dataset_id='99a374e15fd142049e247aee3b973c15';</v>
       </c>
-      <c r="F39" s="0" t="str">
+      <c r="F39" s="1" t="str">
         <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B38&amp;"';"</f>
         <v>--DELETE FROM geohub.dataset_tag WHERE dataset_id='99a374e15fd142049e247aee3b973c15';</v>
       </c>
-      <c r="G39" s="0" t="str">
+      <c r="G39" s="1" t="str">
         <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B38&amp;"';"</f>
         <v>--DELETE FROM geohub.dataset_tag WHERE dataset_id='99a374e15fd142049e247aee3b973c15';</v>
       </c>
-      <c r="I39" s="0" t="str">
-        <f aca="false">""</f>
-        <v/>
-      </c>
-      <c r="K39" s="0" t="str">
+      <c r="I39" s="1" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="K39" s="1" t="str">
         <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B38&amp;"';"</f>
         <v>--DELETE FROM geohub.dataset_tag WHERE dataset_id='99a374e15fd142049e247aee3b973c15';</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I40" s="0" t="str">
+      <c r="I40" s="1" t="str">
         <f aca="false">""</f>
         <v/>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="3" t="str">
+      <c r="B41" s="5" t="str">
         <f aca="false">"echo -n '"&amp;B37&amp;"'|md5sum"</f>
-        <v>echo -n 'http://172.18.0.6:7800/admin.subnational_mean_years_of_schooling/{z}/{x}/{y}.pbf'|md5sum</v>
-      </c>
-      <c r="I41" s="0" t="str">
+        <v>echo -n 'https://pgtileserv.undpgeohub.org/admin.subnational_mean_years_of_schooling/{z}/{x}/{y}.pbf'|md5sum</v>
+      </c>
+      <c r="I41" s="1" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I46" s="1" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B47" s="1" t="str">
+        <f aca="false">$B$1&amp;B46&amp;"/{z}/{x}/{y}.pbf"</f>
+        <v>https://pgtileserv.undpgeohub.org/drr.dynamic_subnational_hhr/{z}/{x}/{y}.pbf</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D47" s="1" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="E47" s="1" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="F47" s="1" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="G47" s="1" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="I47" s="1" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="K47" s="4" t="str">
+        <f aca="false">"INSERT INTO geohub.tag (key, value) SELECT '"&amp;K$3&amp;"', '"&amp;$B46&amp;"' WHERE NOT EXISTS (SELECT key,value FROM geohub.tag WHERE key='"&amp;K$3&amp;"' AND value='"&amp;B46&amp;"');"</f>
+        <v>INSERT INTO geohub.tag (key, value) SELECT 'id', 'drr.dynamic_subnational_hhr' WHERE NOT EXISTS (SELECT key,value FROM geohub.tag WHERE key='id' AND value='drr.dynamic_subnational_hhr');</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C48" s="5" t="str">
+        <f aca="false">"VALUES ('"&amp;B48&amp;"', '"&amp;B47&amp;"', False, 'Creative Commons BY NonCommercial ShareAlike 4.0', (SELECT ST_SetSRID(ST_Extent(geom),4326)  AS geom FROM admin.admin0), current_timestamp, current_timestamp, '"&amp;B49&amp;"', '"&amp;B49&amp;"', 'douglas.tommasi@undp.org', 'douglas.tommasi@undp.org');"</f>
+        <v>VALUES ('8c4810867c50ee006b11abf19876a750', 'https://pgtileserv.undpgeohub.org/drr.dynamic_subnational_hhr/{z}/{x}/{y}.pbf', False, 'Creative Commons BY NonCommercial ShareAlike 4.0', (SELECT ST_SetSRID(ST_Extent(geom),4326)  AS geom FROM admin.admin0), current_timestamp, current_timestamp, 'Subnational Heat Health Risk', 'Subnational Heat Health Risk', 'douglas.tommasi@undp.org', 'douglas.tommasi@undp.org');</v>
+      </c>
+      <c r="D48" s="1" t="str">
+        <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B48&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;D$3&amp;"' AND value='"&amp;D$4&amp;"'))  ON CONFLICT DO NOTHING;"</f>
+        <v>INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('8c4810867c50ee006b11abf19876a750',(SELECT id FROM geohub.tag WHERE key='type' AND value='pgtileserv'))  ON CONFLICT DO NOTHING;</v>
+      </c>
+      <c r="E48" s="1" t="str">
+        <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B48&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;E$3&amp;"' AND value='"&amp;E$4&amp;"'))  ON CONFLICT DO NOTHING;"</f>
+        <v>INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('8c4810867c50ee006b11abf19876a750',(SELECT id FROM geohub.tag WHERE key='layertype' AND value='function'))  ON CONFLICT DO NOTHING;</v>
+      </c>
+      <c r="F48" s="1" t="str">
+        <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B48&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;F$3&amp;"' AND value='"&amp;F$4&amp;"'))  ON CONFLICT DO NOTHING;"</f>
+        <v>INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('8c4810867c50ee006b11abf19876a750',(SELECT id FROM geohub.tag WHERE key='extent' AND value='Global'))  ON CONFLICT DO NOTHING;</v>
+      </c>
+      <c r="G48" s="1" t="str">
+        <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B48&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;G$3&amp;"' AND value='"&amp;G$4&amp;"'))  ON CONFLICT DO NOTHING;"</f>
+        <v>INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('8c4810867c50ee006b11abf19876a750',(SELECT id FROM geohub.tag WHERE key='geometrytype' AND value='MultiPolygon'))  ON CONFLICT DO NOTHING;</v>
+      </c>
+      <c r="I48" s="1" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="K48" s="1" t="str">
+        <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B48&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;K$3&amp;"' AND value='"&amp;$B46&amp;"'))  ON CONFLICT DO NOTHING;"</f>
+        <v>INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('8c4810867c50ee006b11abf19876a750',(SELECT id FROM geohub.tag WHERE key='id' AND value='drr.dynamic_subnational_hhr'))  ON CONFLICT DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C49" s="1" t="str">
+        <f aca="false">"--DELETE FROM geohub.dataset WHERE id ='"&amp;B48&amp;"';"</f>
+        <v>--DELETE FROM geohub.dataset WHERE id ='8c4810867c50ee006b11abf19876a750';</v>
+      </c>
+      <c r="D49" s="1" t="str">
+        <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B48&amp;"';"</f>
+        <v>--DELETE FROM geohub.dataset_tag WHERE dataset_id='8c4810867c50ee006b11abf19876a750';</v>
+      </c>
+      <c r="E49" s="1" t="str">
+        <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B48&amp;"';"</f>
+        <v>--DELETE FROM geohub.dataset_tag WHERE dataset_id='8c4810867c50ee006b11abf19876a750';</v>
+      </c>
+      <c r="F49" s="1" t="str">
+        <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B48&amp;"';"</f>
+        <v>--DELETE FROM geohub.dataset_tag WHERE dataset_id='8c4810867c50ee006b11abf19876a750';</v>
+      </c>
+      <c r="G49" s="1" t="str">
+        <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B48&amp;"';"</f>
+        <v>--DELETE FROM geohub.dataset_tag WHERE dataset_id='8c4810867c50ee006b11abf19876a750';</v>
+      </c>
+      <c r="I49" s="1" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="K49" s="1" t="str">
+        <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B48&amp;"';"</f>
+        <v>--DELETE FROM geohub.dataset_tag WHERE dataset_id='8c4810867c50ee006b11abf19876a750';</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I50" s="1" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="5" t="str">
+        <f aca="false">"echo -n '"&amp;B47&amp;"'|md5sum"</f>
+        <v>echo -n 'https://pgtileserv.undpgeohub.org/drr.dynamic_subnational_hhr/{z}/{x}/{y}.pbf'|md5sum</v>
+      </c>
+      <c r="I51" s="1" t="str">
         <f aca="false">""</f>
         <v/>
       </c>

</xml_diff>

<commit_message>
hrr2 gives correct values
</commit_message>
<xml_diff>
--- a/src/geohubsql/sql/plpgsql/GeoHub_layer_registration.xlsx
+++ b/src/geohubsql/sql/plpgsql/GeoHub_layer_registration.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="35">
   <si>
     <t xml:space="preserve">https://github.com/UNDP-Data/geohub/pull/1556</t>
   </si>
@@ -116,6 +116,15 @@
   </si>
   <si>
     <t xml:space="preserve">Subnational Heat Health Risk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">drr.dynamic_subnational_hhr2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7c8f127000359223747dc870f32a03f9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subnational Heat Health Risk2</t>
   </si>
 </sst>
 </file>
@@ -130,7 +139,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -202,7 +210,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -220,10 +228,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -304,17 +308,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K51"/>
+  <dimension ref="A1:K62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F27" activeCellId="0" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="77.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="92.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="296.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="200.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="200.27"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -432,7 +436,7 @@
       <c r="B8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="5" t="str">
+      <c r="C8" s="1" t="str">
         <f aca="false">"VALUES ('"&amp;B8&amp;"', '"&amp;B7&amp;"', False, 'Creative Commons BY NonCommercial ShareAlike 4.0', (SELECT ST_SetSRID(ST_Extent(geom),4326)  AS geom FROM admin.admin0), current_timestamp, current_timestamp, '"&amp;B9&amp;"', '"&amp;B9&amp;"', 'douglas.tommasi@undp.org', 'douglas.tommasi@undp.org');"</f>
         <v>VALUES ('b35c09fd8fc981d388381dddc146713c', 'https://pgtileserv.undpgeohub.org/admin.subnational_gross_national_income/{z}/{x}/{y}.pbf', False, 'Creative Commons BY NonCommercial ShareAlike 4.0', (SELECT ST_SetSRID(ST_Extent(geom),4326)  AS geom FROM admin.admin0), current_timestamp, current_timestamp, 'Subnational Gross National Income per capita', 'Subnational Gross National Income per capita', 'douglas.tommasi@undp.org', 'douglas.tommasi@undp.org');</v>
       </c>
@@ -504,7 +508,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="5" t="str">
+      <c r="B11" s="1" t="str">
         <f aca="false">"echo -n '"&amp;B7&amp;"'|md5sum"</f>
         <v>echo -n 'https://pgtileserv.undpgeohub.org/admin.subnational_gross_national_income/{z}/{x}/{y}.pbf'|md5sum</v>
       </c>
@@ -598,7 +602,7 @@
       <c r="B19" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="5" t="str">
+      <c r="C19" s="1" t="str">
         <f aca="false">"VALUES ('"&amp;B19&amp;"', '"&amp;B18&amp;"', False, 'Creative Commons BY NonCommercial ShareAlike 4.0', (SELECT ST_SetSRID(ST_Extent(geom),4326)  AS geom FROM admin.admin0), current_timestamp, current_timestamp, '"&amp;B20&amp;"', '"&amp;B20&amp;"', 'douglas.tommasi@undp.org', 'douglas.tommasi@undp.org');"</f>
         <v>VALUES ('3b0a0ed77b9560c8047a9b9c0313cb0a', 'https://pgtileserv.undpgeohub.org/admin.subnational_life_expectancy/{z}/{x}/{y}.pbf', False, 'Creative Commons BY NonCommercial ShareAlike 4.0', (SELECT ST_SetSRID(ST_Extent(geom),4326)  AS geom FROM admin.admin0), current_timestamp, current_timestamp, 'Subnational Life Expectancy', 'Subnational Life Expectancy', 'douglas.tommasi@undp.org', 'douglas.tommasi@undp.org');</v>
       </c>
@@ -670,7 +674,7 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="5" t="str">
+      <c r="B22" s="1" t="str">
         <f aca="false">"echo -n '"&amp;B18&amp;"'|md5sum"</f>
         <v>echo -n 'https://pgtileserv.undpgeohub.org/admin.subnational_life_expectancy/{z}/{x}/{y}.pbf'|md5sum</v>
       </c>
@@ -734,7 +738,7 @@
       <c r="B30" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C30" s="5" t="str">
+      <c r="C30" s="1" t="str">
         <f aca="false">"VALUES ('"&amp;B30&amp;"', '"&amp;B29&amp;"', False, 'Creative Commons BY NonCommercial ShareAlike 4.0', (SELECT ST_SetSRID(ST_Extent(geom),4326)  AS geom FROM admin.admin0), current_timestamp, current_timestamp, '"&amp;B31&amp;"', '"&amp;B31&amp;"', 'douglas.tommasi@undp.org', 'douglas.tommasi@undp.org');"</f>
         <v>VALUES ('571be599e1cc42752265fc7652f296de', 'https://pgtileserv.undpgeohub.org/admin.subnational_expected_years_of_schooling/{z}/{x}/{y}.pbf', False, 'Creative Commons BY NonCommercial ShareAlike 4.0', (SELECT ST_SetSRID(ST_Extent(geom),4326)  AS geom FROM admin.admin0), current_timestamp, current_timestamp, 'Subnational Expected years of schooling', 'Subnational Expected years of schooling', 'douglas.tommasi@undp.org', 'douglas.tommasi@undp.org');</v>
       </c>
@@ -806,7 +810,7 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="5" t="str">
+      <c r="B33" s="1" t="str">
         <f aca="false">"echo -n '"&amp;B29&amp;"'|md5sum"</f>
         <v>echo -n 'https://pgtileserv.undpgeohub.org/admin.subnational_expected_years_of_schooling/{z}/{x}/{y}.pbf'|md5sum</v>
       </c>
@@ -870,7 +874,7 @@
       <c r="B38" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C38" s="5" t="str">
+      <c r="C38" s="1" t="str">
         <f aca="false">"VALUES ('"&amp;B38&amp;"', '"&amp;B37&amp;"', False, 'Creative Commons BY NonCommercial ShareAlike 4.0', (SELECT ST_SetSRID(ST_Extent(geom),4326)  AS geom FROM admin.admin0), current_timestamp, current_timestamp, '"&amp;B39&amp;"', '"&amp;B39&amp;"', 'douglas.tommasi@undp.org', 'douglas.tommasi@undp.org');"</f>
         <v>VALUES ('99a374e15fd142049e247aee3b973c15', 'https://pgtileserv.undpgeohub.org/admin.subnational_mean_years_of_schooling/{z}/{x}/{y}.pbf', False, 'Creative Commons BY NonCommercial ShareAlike 4.0', (SELECT ST_SetSRID(ST_Extent(geom),4326)  AS geom FROM admin.admin0), current_timestamp, current_timestamp, 'Subnational Mean years of schooling', 'Subnational Mean years of schooling', 'douglas.tommasi@undp.org', 'douglas.tommasi@undp.org');</v>
       </c>
@@ -942,7 +946,7 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="5" t="str">
+      <c r="B41" s="1" t="str">
         <f aca="false">"echo -n '"&amp;B37&amp;"'|md5sum"</f>
         <v>echo -n 'https://pgtileserv.undpgeohub.org/admin.subnational_mean_years_of_schooling/{z}/{x}/{y}.pbf'|md5sum</v>
       </c>
@@ -1011,7 +1015,7 @@
       <c r="B48" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C48" s="5" t="str">
+      <c r="C48" s="1" t="str">
         <f aca="false">"VALUES ('"&amp;B48&amp;"', '"&amp;B47&amp;"', False, 'Creative Commons BY NonCommercial ShareAlike 4.0', (SELECT ST_SetSRID(ST_Extent(geom),4326)  AS geom FROM admin.admin0), current_timestamp, current_timestamp, '"&amp;B49&amp;"', '"&amp;B49&amp;"', 'douglas.tommasi@undp.org', 'douglas.tommasi@undp.org');"</f>
         <v>VALUES ('8c4810867c50ee006b11abf19876a750', 'https://pgtileserv.undpgeohub.org/drr.dynamic_subnational_hhr/{z}/{x}/{y}.pbf', False, 'Creative Commons BY NonCommercial ShareAlike 4.0', (SELECT ST_SetSRID(ST_Extent(geom),4326)  AS geom FROM admin.admin0), current_timestamp, current_timestamp, 'Subnational Heat Health Risk', 'Subnational Heat Health Risk', 'douglas.tommasi@undp.org', 'douglas.tommasi@undp.org');</v>
       </c>
@@ -1083,11 +1087,152 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="5" t="str">
+      <c r="B51" s="1" t="str">
         <f aca="false">"echo -n '"&amp;B47&amp;"'|md5sum"</f>
         <v>echo -n 'https://pgtileserv.undpgeohub.org/drr.dynamic_subnational_hhr/{z}/{x}/{y}.pbf'|md5sum</v>
       </c>
       <c r="I51" s="1" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B56" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I57" s="1" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B58" s="1" t="str">
+        <f aca="false">$B$1&amp;B57&amp;"/{z}/{x}/{y}.pbf"</f>
+        <v>https://pgtileserv.undpgeohub.org/drr.dynamic_subnational_hhr2/{z}/{x}/{y}.pbf</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D58" s="1" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="E58" s="1" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="F58" s="1" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="G58" s="1" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="I58" s="1" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="K58" s="4" t="str">
+        <f aca="false">"INSERT INTO geohub.tag (key, value) SELECT '"&amp;K$3&amp;"', '"&amp;$B57&amp;"' WHERE NOT EXISTS (SELECT key,value FROM geohub.tag WHERE key='"&amp;K$3&amp;"' AND value='"&amp;B57&amp;"');"</f>
+        <v>INSERT INTO geohub.tag (key, value) SELECT 'id', 'drr.dynamic_subnational_hhr2' WHERE NOT EXISTS (SELECT key,value FROM geohub.tag WHERE key='id' AND value='drr.dynamic_subnational_hhr2');</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C59" s="1" t="str">
+        <f aca="false">"VALUES ('"&amp;B59&amp;"', '"&amp;B58&amp;"', False, 'Creative Commons BY NonCommercial ShareAlike 4.0', (SELECT ST_SetSRID(ST_Extent(geom),4326)  AS geom FROM admin.admin0), current_timestamp, current_timestamp, '"&amp;B60&amp;"', '"&amp;B60&amp;"', 'douglas.tommasi@undp.org', 'douglas.tommasi@undp.org');"</f>
+        <v>VALUES ('7c8f127000359223747dc870f32a03f9', 'https://pgtileserv.undpgeohub.org/drr.dynamic_subnational_hhr2/{z}/{x}/{y}.pbf', False, 'Creative Commons BY NonCommercial ShareAlike 4.0', (SELECT ST_SetSRID(ST_Extent(geom),4326)  AS geom FROM admin.admin0), current_timestamp, current_timestamp, 'Subnational Heat Health Risk2', 'Subnational Heat Health Risk2', 'douglas.tommasi@undp.org', 'douglas.tommasi@undp.org');</v>
+      </c>
+      <c r="D59" s="1" t="str">
+        <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B59&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;D$3&amp;"' AND value='"&amp;D$4&amp;"'))  ON CONFLICT DO NOTHING;"</f>
+        <v>INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('7c8f127000359223747dc870f32a03f9',(SELECT id FROM geohub.tag WHERE key='type' AND value='pgtileserv'))  ON CONFLICT DO NOTHING;</v>
+      </c>
+      <c r="E59" s="1" t="str">
+        <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B59&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;E$3&amp;"' AND value='"&amp;E$4&amp;"'))  ON CONFLICT DO NOTHING;"</f>
+        <v>INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('7c8f127000359223747dc870f32a03f9',(SELECT id FROM geohub.tag WHERE key='layertype' AND value='function'))  ON CONFLICT DO NOTHING;</v>
+      </c>
+      <c r="F59" s="1" t="str">
+        <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B59&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;F$3&amp;"' AND value='"&amp;F$4&amp;"'))  ON CONFLICT DO NOTHING;"</f>
+        <v>INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('7c8f127000359223747dc870f32a03f9',(SELECT id FROM geohub.tag WHERE key='extent' AND value='Global'))  ON CONFLICT DO NOTHING;</v>
+      </c>
+      <c r="G59" s="1" t="str">
+        <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B59&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;G$3&amp;"' AND value='"&amp;G$4&amp;"'))  ON CONFLICT DO NOTHING;"</f>
+        <v>INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('7c8f127000359223747dc870f32a03f9',(SELECT id FROM geohub.tag WHERE key='geometrytype' AND value='MultiPolygon'))  ON CONFLICT DO NOTHING;</v>
+      </c>
+      <c r="I59" s="1" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="K59" s="1" t="str">
+        <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B59&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;K$3&amp;"' AND value='"&amp;$B57&amp;"'))  ON CONFLICT DO NOTHING;"</f>
+        <v>INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('7c8f127000359223747dc870f32a03f9',(SELECT id FROM geohub.tag WHERE key='id' AND value='drr.dynamic_subnational_hhr2'))  ON CONFLICT DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C60" s="1" t="str">
+        <f aca="false">"--DELETE FROM geohub.dataset WHERE id ='"&amp;B59&amp;"';"</f>
+        <v>--DELETE FROM geohub.dataset WHERE id ='7c8f127000359223747dc870f32a03f9';</v>
+      </c>
+      <c r="D60" s="1" t="str">
+        <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B59&amp;"';"</f>
+        <v>--DELETE FROM geohub.dataset_tag WHERE dataset_id='7c8f127000359223747dc870f32a03f9';</v>
+      </c>
+      <c r="E60" s="1" t="str">
+        <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B59&amp;"';"</f>
+        <v>--DELETE FROM geohub.dataset_tag WHERE dataset_id='7c8f127000359223747dc870f32a03f9';</v>
+      </c>
+      <c r="F60" s="1" t="str">
+        <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B59&amp;"';"</f>
+        <v>--DELETE FROM geohub.dataset_tag WHERE dataset_id='7c8f127000359223747dc870f32a03f9';</v>
+      </c>
+      <c r="G60" s="1" t="str">
+        <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B59&amp;"';"</f>
+        <v>--DELETE FROM geohub.dataset_tag WHERE dataset_id='7c8f127000359223747dc870f32a03f9';</v>
+      </c>
+      <c r="I60" s="1" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="K60" s="1" t="str">
+        <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B59&amp;"';"</f>
+        <v>--DELETE FROM geohub.dataset_tag WHERE dataset_id='7c8f127000359223747dc870f32a03f9';</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I61" s="1" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B62" s="1" t="str">
+        <f aca="false">"echo -n '"&amp;B58&amp;"'|md5sum"</f>
+        <v>echo -n 'https://pgtileserv.undpgeohub.org/drr.dynamic_subnational_hhr2/{z}/{x}/{y}.pbf'|md5sum</v>
+      </c>
+      <c r="I62" s="1" t="str">
         <f aca="false">""</f>
         <v/>
       </c>

</xml_diff>

<commit_message>
refactored 'dynamic_subnational_hhr' back into 'dynamic_subnational_hhr', added some tags to the registration excel
</commit_message>
<xml_diff>
--- a/src/geohubsql/sql/plpgsql/GeoHub_layer_registration.xlsx
+++ b/src/geohubsql/sql/plpgsql/GeoHub_layer_registration.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="43">
   <si>
     <t xml:space="preserve">https://github.com/UNDP-Data/geohub/pull/1556</t>
   </si>
@@ -40,6 +40,12 @@
     <t xml:space="preserve">geometrytype</t>
   </si>
   <si>
+    <t xml:space="preserve">granularity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provider</t>
+  </si>
+  <si>
     <t xml:space="preserve">id</t>
   </si>
   <si>
@@ -58,6 +64,12 @@
     <t xml:space="preserve">MultiPolygon</t>
   </si>
   <si>
+    <t xml:space="preserve">admin1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">United Nations Development Programme (UNDP)</t>
+  </si>
+  <si>
     <t xml:space="preserve">function name</t>
   </si>
   <si>
@@ -125,6 +137,18 @@
   </si>
   <si>
     <t xml:space="preserve">Subnational Heat Health Risk2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT dt.*, t.value, t.key </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FROM geohub.dataset_tag AS dt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JOIN geohub.tag t ON t.id = dt.tag_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WHERE dataset_id='8c4810867c50ee006b11abf19876a750' OR dataset_id='7c8f127000359223747dc870f32a03f9';</t>
   </si>
 </sst>
 </file>
@@ -139,6 +163,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -308,16 +333,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K62"/>
+  <dimension ref="A1:K74"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F27" activeCellId="0" sqref="F27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H59" activeCellId="0" sqref="H59:I60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="92.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="296.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="181.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="200.27"/>
   </cols>
   <sheetData>
@@ -346,33 +372,37 @@
       <c r="G3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="1" t="str">
-        <f aca="false">""</f>
-        <v/>
+      <c r="H3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="1" t="str">
-        <f aca="false">""</f>
-        <v/>
+        <v>13</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -383,10 +413,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="I6" s="1" t="str">
         <f aca="false">""</f>
@@ -395,14 +425,14 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B7" s="1" t="str">
         <f aca="false">$B$1&amp;B6&amp;"/{z}/{x}/{y}.pbf"</f>
         <v>https://pgtileserv.undpgeohub.org/admin.subnational_gross_national_income/{z}/{x}/{y}.pbf</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D7" s="1" t="str">
         <f aca="false">""</f>
@@ -431,10 +461,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C8" s="1" t="str">
         <f aca="false">"VALUES ('"&amp;B8&amp;"', '"&amp;B7&amp;"', False, 'Creative Commons BY NonCommercial ShareAlike 4.0', (SELECT ST_SetSRID(ST_Extent(geom),4326)  AS geom FROM admin.admin0), current_timestamp, current_timestamp, '"&amp;B9&amp;"', '"&amp;B9&amp;"', 'douglas.tommasi@undp.org', 'douglas.tommasi@undp.org');"</f>
@@ -456,9 +486,13 @@
         <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B8&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;G$3&amp;"' AND value='"&amp;G$4&amp;"'))  ON CONFLICT DO NOTHING;"</f>
         <v>INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('b35c09fd8fc981d388381dddc146713c',(SELECT id FROM geohub.tag WHERE key='geometrytype' AND value='MultiPolygon'))  ON CONFLICT DO NOTHING;</v>
       </c>
+      <c r="H8" s="1" t="str">
+        <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B8&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;H$3&amp;"' AND value='"&amp;H$4&amp;"'))  ON CONFLICT DO NOTHING;"</f>
+        <v>INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('b35c09fd8fc981d388381dddc146713c',(SELECT id FROM geohub.tag WHERE key='granularity' AND value='admin1'))  ON CONFLICT DO NOTHING;</v>
+      </c>
       <c r="I8" s="1" t="str">
-        <f aca="false">""</f>
-        <v/>
+        <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B8&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;I$3&amp;"' AND value='"&amp;I$4&amp;"'))  ON CONFLICT DO NOTHING;"</f>
+        <v>INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('b35c09fd8fc981d388381dddc146713c',(SELECT id FROM geohub.tag WHERE key='provider' AND value='United Nations Development Programme (UNDP)'))  ON CONFLICT DO NOTHING;</v>
       </c>
       <c r="K8" s="1" t="str">
         <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B8&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;K$3&amp;"' AND value='"&amp;$B6&amp;"'))  ON CONFLICT DO NOTHING;"</f>
@@ -467,10 +501,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C9" s="1" t="str">
         <f aca="false">"--DELETE FROM geohub.dataset WHERE id ='"&amp;B8&amp;"';"</f>
@@ -492,9 +526,13 @@
         <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B8&amp;"';"</f>
         <v>--DELETE FROM geohub.dataset_tag WHERE dataset_id='b35c09fd8fc981d388381dddc146713c';</v>
       </c>
+      <c r="H9" s="1" t="str">
+        <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B8&amp;"';"</f>
+        <v>--DELETE FROM geohub.dataset_tag WHERE dataset_id='b35c09fd8fc981d388381dddc146713c';</v>
+      </c>
       <c r="I9" s="1" t="str">
-        <f aca="false">""</f>
-        <v/>
+        <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B8&amp;"';"</f>
+        <v>--DELETE FROM geohub.dataset_tag WHERE dataset_id='b35c09fd8fc981d388381dddc146713c';</v>
       </c>
       <c r="K9" s="1" t="str">
         <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B8&amp;"';"</f>
@@ -549,10 +587,10 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="I17" s="1" t="str">
         <f aca="false">""</f>
@@ -561,14 +599,14 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B18" s="1" t="str">
         <f aca="false">$B$1&amp;B17&amp;"/{z}/{x}/{y}.pbf"</f>
         <v>https://pgtileserv.undpgeohub.org/admin.subnational_life_expectancy/{z}/{x}/{y}.pbf</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D18" s="1" t="str">
         <f aca="false">""</f>
@@ -597,10 +635,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C19" s="1" t="str">
         <f aca="false">"VALUES ('"&amp;B19&amp;"', '"&amp;B18&amp;"', False, 'Creative Commons BY NonCommercial ShareAlike 4.0', (SELECT ST_SetSRID(ST_Extent(geom),4326)  AS geom FROM admin.admin0), current_timestamp, current_timestamp, '"&amp;B20&amp;"', '"&amp;B20&amp;"', 'douglas.tommasi@undp.org', 'douglas.tommasi@undp.org');"</f>
@@ -622,9 +660,13 @@
         <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B19&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;G$3&amp;"' AND value='"&amp;G$4&amp;"'))  ON CONFLICT DO NOTHING;"</f>
         <v>INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('3b0a0ed77b9560c8047a9b9c0313cb0a',(SELECT id FROM geohub.tag WHERE key='geometrytype' AND value='MultiPolygon'))  ON CONFLICT DO NOTHING;</v>
       </c>
+      <c r="H19" s="1" t="str">
+        <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B19&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;H$3&amp;"' AND value='"&amp;H$4&amp;"'))  ON CONFLICT DO NOTHING;"</f>
+        <v>INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('3b0a0ed77b9560c8047a9b9c0313cb0a',(SELECT id FROM geohub.tag WHERE key='granularity' AND value='admin1'))  ON CONFLICT DO NOTHING;</v>
+      </c>
       <c r="I19" s="1" t="str">
-        <f aca="false">""</f>
-        <v/>
+        <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B19&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;I$3&amp;"' AND value='"&amp;I$4&amp;"'))  ON CONFLICT DO NOTHING;"</f>
+        <v>INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('3b0a0ed77b9560c8047a9b9c0313cb0a',(SELECT id FROM geohub.tag WHERE key='provider' AND value='United Nations Development Programme (UNDP)'))  ON CONFLICT DO NOTHING;</v>
       </c>
       <c r="K19" s="1" t="str">
         <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B19&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;K$3&amp;"' AND value='"&amp;$B17&amp;"'))  ON CONFLICT DO NOTHING;"</f>
@@ -633,10 +675,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C20" s="1" t="str">
         <f aca="false">"--DELETE FROM geohub.dataset WHERE id ='"&amp;B19&amp;"';"</f>
@@ -658,9 +700,13 @@
         <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B19&amp;"';"</f>
         <v>--DELETE FROM geohub.dataset_tag WHERE dataset_id='3b0a0ed77b9560c8047a9b9c0313cb0a';</v>
       </c>
+      <c r="H20" s="1" t="str">
+        <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B19&amp;"';"</f>
+        <v>--DELETE FROM geohub.dataset_tag WHERE dataset_id='3b0a0ed77b9560c8047a9b9c0313cb0a';</v>
+      </c>
       <c r="I20" s="1" t="str">
-        <f aca="false">""</f>
-        <v/>
+        <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B19&amp;"';"</f>
+        <v>--DELETE FROM geohub.dataset_tag WHERE dataset_id='3b0a0ed77b9560c8047a9b9c0313cb0a';</v>
       </c>
       <c r="K20" s="1" t="str">
         <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B19&amp;"';"</f>
@@ -685,10 +731,10 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="I28" s="1" t="str">
         <f aca="false">""</f>
@@ -697,14 +743,14 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B29" s="1" t="str">
         <f aca="false">$B$1&amp;B28&amp;"/{z}/{x}/{y}.pbf"</f>
         <v>https://pgtileserv.undpgeohub.org/admin.subnational_expected_years_of_schooling/{z}/{x}/{y}.pbf</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D29" s="1" t="str">
         <f aca="false">""</f>
@@ -733,10 +779,10 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C30" s="1" t="str">
         <f aca="false">"VALUES ('"&amp;B30&amp;"', '"&amp;B29&amp;"', False, 'Creative Commons BY NonCommercial ShareAlike 4.0', (SELECT ST_SetSRID(ST_Extent(geom),4326)  AS geom FROM admin.admin0), current_timestamp, current_timestamp, '"&amp;B31&amp;"', '"&amp;B31&amp;"', 'douglas.tommasi@undp.org', 'douglas.tommasi@undp.org');"</f>
@@ -758,9 +804,13 @@
         <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B30&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;G$3&amp;"' AND value='"&amp;G$4&amp;"'))  ON CONFLICT DO NOTHING;"</f>
         <v>INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('571be599e1cc42752265fc7652f296de',(SELECT id FROM geohub.tag WHERE key='geometrytype' AND value='MultiPolygon'))  ON CONFLICT DO NOTHING;</v>
       </c>
+      <c r="H30" s="1" t="str">
+        <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B30&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;H$3&amp;"' AND value='"&amp;H$4&amp;"'))  ON CONFLICT DO NOTHING;"</f>
+        <v>INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('571be599e1cc42752265fc7652f296de',(SELECT id FROM geohub.tag WHERE key='granularity' AND value='admin1'))  ON CONFLICT DO NOTHING;</v>
+      </c>
       <c r="I30" s="1" t="str">
-        <f aca="false">""</f>
-        <v/>
+        <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B30&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;I$3&amp;"' AND value='"&amp;I$4&amp;"'))  ON CONFLICT DO NOTHING;"</f>
+        <v>INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('571be599e1cc42752265fc7652f296de',(SELECT id FROM geohub.tag WHERE key='provider' AND value='United Nations Development Programme (UNDP)'))  ON CONFLICT DO NOTHING;</v>
       </c>
       <c r="K30" s="1" t="str">
         <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B30&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;K$3&amp;"' AND value='"&amp;$B28&amp;"'))  ON CONFLICT DO NOTHING;"</f>
@@ -769,10 +819,10 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C31" s="1" t="str">
         <f aca="false">"--DELETE FROM geohub.dataset WHERE id ='"&amp;B30&amp;"';"</f>
@@ -794,9 +844,13 @@
         <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B30&amp;"';"</f>
         <v>--DELETE FROM geohub.dataset_tag WHERE dataset_id='571be599e1cc42752265fc7652f296de';</v>
       </c>
+      <c r="H31" s="1" t="str">
+        <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B30&amp;"';"</f>
+        <v>--DELETE FROM geohub.dataset_tag WHERE dataset_id='571be599e1cc42752265fc7652f296de';</v>
+      </c>
       <c r="I31" s="1" t="str">
-        <f aca="false">""</f>
-        <v/>
+        <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B30&amp;"';"</f>
+        <v>--DELETE FROM geohub.dataset_tag WHERE dataset_id='571be599e1cc42752265fc7652f296de';</v>
       </c>
       <c r="K31" s="1" t="str">
         <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B30&amp;"';"</f>
@@ -821,10 +875,10 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="I36" s="1" t="str">
         <f aca="false">""</f>
@@ -833,14 +887,14 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B37" s="1" t="str">
         <f aca="false">$B$1&amp;B36&amp;"/{z}/{x}/{y}.pbf"</f>
         <v>https://pgtileserv.undpgeohub.org/admin.subnational_mean_years_of_schooling/{z}/{x}/{y}.pbf</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D37" s="1" t="str">
         <f aca="false">""</f>
@@ -869,10 +923,10 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C38" s="1" t="str">
         <f aca="false">"VALUES ('"&amp;B38&amp;"', '"&amp;B37&amp;"', False, 'Creative Commons BY NonCommercial ShareAlike 4.0', (SELECT ST_SetSRID(ST_Extent(geom),4326)  AS geom FROM admin.admin0), current_timestamp, current_timestamp, '"&amp;B39&amp;"', '"&amp;B39&amp;"', 'douglas.tommasi@undp.org', 'douglas.tommasi@undp.org');"</f>
@@ -894,9 +948,13 @@
         <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B38&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;G$3&amp;"' AND value='"&amp;G$4&amp;"'))  ON CONFLICT DO NOTHING;"</f>
         <v>INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('99a374e15fd142049e247aee3b973c15',(SELECT id FROM geohub.tag WHERE key='geometrytype' AND value='MultiPolygon'))  ON CONFLICT DO NOTHING;</v>
       </c>
+      <c r="H38" s="1" t="str">
+        <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B38&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;H$3&amp;"' AND value='"&amp;H$4&amp;"'))  ON CONFLICT DO NOTHING;"</f>
+        <v>INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('99a374e15fd142049e247aee3b973c15',(SELECT id FROM geohub.tag WHERE key='granularity' AND value='admin1'))  ON CONFLICT DO NOTHING;</v>
+      </c>
       <c r="I38" s="1" t="str">
-        <f aca="false">""</f>
-        <v/>
+        <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B38&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;I$3&amp;"' AND value='"&amp;I$4&amp;"'))  ON CONFLICT DO NOTHING;"</f>
+        <v>INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('99a374e15fd142049e247aee3b973c15',(SELECT id FROM geohub.tag WHERE key='provider' AND value='United Nations Development Programme (UNDP)'))  ON CONFLICT DO NOTHING;</v>
       </c>
       <c r="K38" s="1" t="str">
         <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B38&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;K$3&amp;"' AND value='"&amp;$B36&amp;"'))  ON CONFLICT DO NOTHING;"</f>
@@ -905,10 +963,10 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C39" s="1" t="str">
         <f aca="false">"--DELETE FROM geohub.dataset WHERE id ='"&amp;B38&amp;"';"</f>
@@ -930,9 +988,13 @@
         <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B38&amp;"';"</f>
         <v>--DELETE FROM geohub.dataset_tag WHERE dataset_id='99a374e15fd142049e247aee3b973c15';</v>
       </c>
+      <c r="H39" s="1" t="str">
+        <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B38&amp;"';"</f>
+        <v>--DELETE FROM geohub.dataset_tag WHERE dataset_id='99a374e15fd142049e247aee3b973c15';</v>
+      </c>
       <c r="I39" s="1" t="str">
-        <f aca="false">""</f>
-        <v/>
+        <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B38&amp;"';"</f>
+        <v>--DELETE FROM geohub.dataset_tag WHERE dataset_id='99a374e15fd142049e247aee3b973c15';</v>
       </c>
       <c r="K39" s="1" t="str">
         <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B38&amp;"';"</f>
@@ -957,15 +1019,15 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="I46" s="1" t="str">
         <f aca="false">""</f>
@@ -974,14 +1036,14 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B47" s="1" t="str">
         <f aca="false">$B$1&amp;B46&amp;"/{z}/{x}/{y}.pbf"</f>
         <v>https://pgtileserv.undpgeohub.org/drr.dynamic_subnational_hhr/{z}/{x}/{y}.pbf</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D47" s="1" t="str">
         <f aca="false">""</f>
@@ -1010,10 +1072,10 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C48" s="1" t="str">
         <f aca="false">"VALUES ('"&amp;B48&amp;"', '"&amp;B47&amp;"', False, 'Creative Commons BY NonCommercial ShareAlike 4.0', (SELECT ST_SetSRID(ST_Extent(geom),4326)  AS geom FROM admin.admin0), current_timestamp, current_timestamp, '"&amp;B49&amp;"', '"&amp;B49&amp;"', 'douglas.tommasi@undp.org', 'douglas.tommasi@undp.org');"</f>
@@ -1035,9 +1097,13 @@
         <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B48&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;G$3&amp;"' AND value='"&amp;G$4&amp;"'))  ON CONFLICT DO NOTHING;"</f>
         <v>INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('8c4810867c50ee006b11abf19876a750',(SELECT id FROM geohub.tag WHERE key='geometrytype' AND value='MultiPolygon'))  ON CONFLICT DO NOTHING;</v>
       </c>
+      <c r="H48" s="1" t="str">
+        <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B48&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;H$3&amp;"' AND value='"&amp;H$4&amp;"'))  ON CONFLICT DO NOTHING;"</f>
+        <v>INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('8c4810867c50ee006b11abf19876a750',(SELECT id FROM geohub.tag WHERE key='granularity' AND value='admin1'))  ON CONFLICT DO NOTHING;</v>
+      </c>
       <c r="I48" s="1" t="str">
-        <f aca="false">""</f>
-        <v/>
+        <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B48&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;I$3&amp;"' AND value='"&amp;I$4&amp;"'))  ON CONFLICT DO NOTHING;"</f>
+        <v>INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('8c4810867c50ee006b11abf19876a750',(SELECT id FROM geohub.tag WHERE key='provider' AND value='United Nations Development Programme (UNDP)'))  ON CONFLICT DO NOTHING;</v>
       </c>
       <c r="K48" s="1" t="str">
         <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B48&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;K$3&amp;"' AND value='"&amp;$B46&amp;"'))  ON CONFLICT DO NOTHING;"</f>
@@ -1046,10 +1112,10 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C49" s="1" t="str">
         <f aca="false">"--DELETE FROM geohub.dataset WHERE id ='"&amp;B48&amp;"';"</f>
@@ -1071,9 +1137,13 @@
         <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B48&amp;"';"</f>
         <v>--DELETE FROM geohub.dataset_tag WHERE dataset_id='8c4810867c50ee006b11abf19876a750';</v>
       </c>
+      <c r="H49" s="1" t="str">
+        <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B48&amp;"';"</f>
+        <v>--DELETE FROM geohub.dataset_tag WHERE dataset_id='8c4810867c50ee006b11abf19876a750';</v>
+      </c>
       <c r="I49" s="1" t="str">
-        <f aca="false">""</f>
-        <v/>
+        <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B48&amp;"';"</f>
+        <v>--DELETE FROM geohub.dataset_tag WHERE dataset_id='8c4810867c50ee006b11abf19876a750';</v>
       </c>
       <c r="K49" s="1" t="str">
         <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B48&amp;"';"</f>
@@ -1098,15 +1168,15 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="I57" s="1" t="str">
         <f aca="false">""</f>
@@ -1115,14 +1185,14 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B58" s="1" t="str">
         <f aca="false">$B$1&amp;B57&amp;"/{z}/{x}/{y}.pbf"</f>
         <v>https://pgtileserv.undpgeohub.org/drr.dynamic_subnational_hhr2/{z}/{x}/{y}.pbf</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D58" s="1" t="str">
         <f aca="false">""</f>
@@ -1151,10 +1221,10 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C59" s="1" t="str">
         <f aca="false">"VALUES ('"&amp;B59&amp;"', '"&amp;B58&amp;"', False, 'Creative Commons BY NonCommercial ShareAlike 4.0', (SELECT ST_SetSRID(ST_Extent(geom),4326)  AS geom FROM admin.admin0), current_timestamp, current_timestamp, '"&amp;B60&amp;"', '"&amp;B60&amp;"', 'douglas.tommasi@undp.org', 'douglas.tommasi@undp.org');"</f>
@@ -1176,9 +1246,13 @@
         <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B59&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;G$3&amp;"' AND value='"&amp;G$4&amp;"'))  ON CONFLICT DO NOTHING;"</f>
         <v>INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('7c8f127000359223747dc870f32a03f9',(SELECT id FROM geohub.tag WHERE key='geometrytype' AND value='MultiPolygon'))  ON CONFLICT DO NOTHING;</v>
       </c>
+      <c r="H59" s="1" t="str">
+        <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B59&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;H$3&amp;"' AND value='"&amp;H$4&amp;"'))  ON CONFLICT DO NOTHING;"</f>
+        <v>INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('7c8f127000359223747dc870f32a03f9',(SELECT id FROM geohub.tag WHERE key='granularity' AND value='admin1'))  ON CONFLICT DO NOTHING;</v>
+      </c>
       <c r="I59" s="1" t="str">
-        <f aca="false">""</f>
-        <v/>
+        <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B59&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;I$3&amp;"' AND value='"&amp;I$4&amp;"'))  ON CONFLICT DO NOTHING;"</f>
+        <v>INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('7c8f127000359223747dc870f32a03f9',(SELECT id FROM geohub.tag WHERE key='provider' AND value='United Nations Development Programme (UNDP)'))  ON CONFLICT DO NOTHING;</v>
       </c>
       <c r="K59" s="1" t="str">
         <f aca="false">"INSERT INTO geohub.dataset_tag (dataset_id, tag_id) VALUES ('"&amp;$B59&amp;"',(SELECT id FROM geohub.tag WHERE key='"&amp;K$3&amp;"' AND value='"&amp;$B57&amp;"'))  ON CONFLICT DO NOTHING;"</f>
@@ -1187,10 +1261,10 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C60" s="1" t="str">
         <f aca="false">"--DELETE FROM geohub.dataset WHERE id ='"&amp;B59&amp;"';"</f>
@@ -1212,9 +1286,13 @@
         <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B59&amp;"';"</f>
         <v>--DELETE FROM geohub.dataset_tag WHERE dataset_id='7c8f127000359223747dc870f32a03f9';</v>
       </c>
+      <c r="H60" s="1" t="str">
+        <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B59&amp;"';"</f>
+        <v>--DELETE FROM geohub.dataset_tag WHERE dataset_id='7c8f127000359223747dc870f32a03f9';</v>
+      </c>
       <c r="I60" s="1" t="str">
-        <f aca="false">""</f>
-        <v/>
+        <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B59&amp;"';"</f>
+        <v>--DELETE FROM geohub.dataset_tag WHERE dataset_id='7c8f127000359223747dc870f32a03f9';</v>
       </c>
       <c r="K60" s="1" t="str">
         <f aca="false">"--DELETE FROM geohub.dataset_tag WHERE dataset_id='"&amp;$B59&amp;"';"</f>
@@ -1235,6 +1313,26 @@
       <c r="I62" s="1" t="str">
         <f aca="false">""</f>
         <v/>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B71" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B72" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B73" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B74" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added some handy queries in the GeoHub_layer_registration xlsx
</commit_message>
<xml_diff>
--- a/src/geohubsql/sql/plpgsql/GeoHub_layer_registration.xlsx
+++ b/src/geohubsql/sql/plpgsql/GeoHub_layer_registration.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="44">
   <si>
     <t xml:space="preserve">https://github.com/UNDP-Data/geohub/pull/1556</t>
   </si>
@@ -149,6 +149,9 @@
   </si>
   <si>
     <t xml:space="preserve">WHERE dataset_id='8c4810867c50ee006b11abf19876a750' OR dataset_id='7c8f127000359223747dc870f32a03f9';</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select * from geohub.dataset where name like '%hdi%' LIMIT 5</t>
   </si>
 </sst>
 </file>
@@ -333,17 +336,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K74"/>
+  <dimension ref="A1:K77"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H59" activeCellId="0" sqref="H59:I60"/>
+      <selection pane="topLeft" activeCell="B79" activeCellId="0" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="92.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="181.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="108.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="181.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="22.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="200.27"/>
   </cols>
   <sheetData>
@@ -372,7 +376,7 @@
       <c r="G3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="H3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="I3" s="1" t="s">
@@ -398,7 +402,7 @@
       <c r="G4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="0" t="s">
+      <c r="H4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="I4" s="1" t="s">
@@ -1333,6 +1337,11 @@
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="1" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B77" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>